<commit_message>
add embedding for frat depth2
</commit_message>
<xml_diff>
--- a/output/frat/depth_2/frat_3_conceptnet_search.xlsx
+++ b/output/frat/depth_2/frat_3_conceptnet_search.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rejna/projects/github.com/r_m_thesis/output/frat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\r_m_thesis\output\frat\depth_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C5AC24-A90C-DC47-97FF-4AF548950B3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47722E02-350F-4CF8-AF4E-2CB2134834E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13360" yWindow="500" windowWidth="15980" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1227,19 +1227,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="29.36328125" customWidth="1"/>
+    <col min="2" max="2" width="35.6328125" customWidth="1"/>
     <col min="3" max="3" width="35" customWidth="1"/>
     <col min="4" max="4" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1437,7 +1437,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1529,7 +1529,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1897,7 +1897,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1931,7 +1931,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1945,7 +1945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -2085,7 +2085,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -2131,7 +2131,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H50" t="s">
         <v>267</v>
       </c>

</xml_diff>

<commit_message>
update names + task
</commit_message>
<xml_diff>
--- a/output/frat/depth_2/frat_3_conceptnet_search.xlsx
+++ b/output/frat/depth_2/frat_3_conceptnet_search.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rejna/projects/github.com/r_m_thesis/output/frat/depth_2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C36B7BC-8DEA-5F46-A31F-313F53FE17B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -703,8 +709,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -767,6 +773,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -813,7 +827,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -845,9 +859,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -879,6 +911,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1054,14 +1104,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1087,7 +1144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1107,7 +1164,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1127,7 +1184,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1204,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1167,7 +1224,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1187,7 +1244,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1198,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1218,7 +1275,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1238,7 +1295,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1258,7 +1315,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1278,7 +1335,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1298,7 +1355,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1318,7 +1375,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1338,7 +1395,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1358,7 +1415,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1378,7 +1435,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -1398,7 +1455,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1418,7 +1475,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1438,7 +1495,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1458,7 +1515,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1478,7 +1535,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1498,7 +1555,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1518,7 +1575,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1538,7 +1595,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1558,7 +1615,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1578,7 +1635,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1598,7 +1655,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -1618,7 +1675,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1638,7 +1695,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1649,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1669,7 +1726,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1683,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1703,7 +1760,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1723,7 +1780,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1734,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1754,7 +1811,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1774,7 +1831,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1788,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -1808,7 +1865,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>46</v>
       </c>
@@ -1828,7 +1885,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>47</v>
       </c>
@@ -1848,7 +1905,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>48</v>
       </c>
@@ -1868,7 +1925,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>49</v>
       </c>
@@ -1888,7 +1945,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -1908,7 +1965,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -1928,7 +1985,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -1942,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>53</v>
       </c>
@@ -1962,7 +2019,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>54</v>
       </c>
@@ -1976,7 +2033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1990,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H50" t="s">
         <v>227</v>
       </c>

</xml_diff>